<commit_message>
Research Tree (Continued) - 3030499331 업데이트
</commit_message>
<xml_diff>
--- a/Data/Mlie/Research Tree (Continued) - 3030499331/3030499331.xlsx
+++ b/Data/Mlie/Research Tree (Continued) - 3030499331/3030499331.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.9.1\Research Tree (Continued) - 3030499331\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Research Tree (Continued) - 3030499331\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055BD0CE-C4FF-4376-AAF8-01376D4BE052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659C6D3B-5EE4-43DC-9604-3C397C95BC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="38340" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240627" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,724 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>bjmi0</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-07-16</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>삭제됨</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>삭제</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이전</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>번역문</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>: '</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>연구</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-07-16</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>삭제됨</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>삭제</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이전</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>번역문</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>: '</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>가능한</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>연구</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>목록을</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>확인하고</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>연구과제를</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>정합니다</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.\n\nShift+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>클릭으로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>기본</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>연구</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> UI</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>를</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>열</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>수</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>있습니다</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>.'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-07-16에 삭제됨. 삭제 이전 번역문: '연구'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-07-16에 삭제됨. 삭제 이전 번역문: '가능한 연구 목록을 확인하고 연구과제를 정합니다.'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-07-16 이전의 원문: 'Left-Click to remove from queue'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-07-16</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>에</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>삭제됨</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">. </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>삭제</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이전</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>번역문</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>: '</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>요구</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>사항</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-07-16에 삭제됨. 삭제 이전 번역문: '선행 기술'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-07-16에 삭제됨. 삭제 이전 번역문: '이전 그래픽 방식 사용 (깜박이는 경우)'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E54" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-07-16에 새로 추가된 노드들 (18개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="270">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -65,6 +781,9 @@
     <t>research</t>
   </si>
   <si>
+    <t>Keyed+Fluffy.ResearchTree.HoldForClassic</t>
+  </si>
+  <si>
     <t>MainButtonDef+Research.description</t>
   </si>
   <si>
@@ -74,6 +793,9 @@
     <t>Examine and decide on research projects.\n\nShift+click to open the original tree.</t>
   </si>
   <si>
+    <t>Fluffy.ResearchTree.HoldForClassic</t>
+  </si>
+  <si>
     <t>MainButtonDef+ResearchOriginal.label</t>
   </si>
   <si>
@@ -89,6 +811,9 @@
     <t>Examine and decide on research projects.</t>
   </si>
   <si>
+    <t>FluffyResearchTree.description</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.AllowsBuildingX</t>
   </si>
   <si>
@@ -101,6 +826,9 @@
     <t>Enables construction {0}</t>
   </si>
   <si>
+    <t>{0} 건설 사용 가능</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.AllowsCraftingX</t>
   </si>
   <si>
@@ -110,6 +838,9 @@
     <t>Enables recipe {0}</t>
   </si>
   <si>
+    <t>{0} 레시피 사용 가능</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.AllowsSowingXinY</t>
   </si>
   <si>
@@ -122,12 +853,27 @@
     <t>Keyed+Fluffy.ResearchTree.AllowsPlantingX</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>{0}(을)를 {1}에 심기 가능</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Fluffy.ResearchTree.AllowsPlantingX</t>
   </si>
   <si>
     <t>Enables growing {0}</t>
   </si>
   <si>
+    <t>{0} 재배 가능</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.LClickReplaceQueue</t>
   </si>
   <si>
@@ -137,13 +883,16 @@
     <t>Left-Click to replace queue</t>
   </si>
   <si>
+    <t>왼쪽 클릭으로 대기열을 변경합니다.</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.LClickRemoveFromQueue</t>
   </si>
   <si>
     <t>Fluffy.ResearchTree.LClickRemoveFromQueue</t>
   </si>
   <si>
-    <t>Left-Click to remove from queue</t>
+    <t>MainButtonDef+FluffyResearchTree.label</t>
   </si>
   <si>
     <t>Keyed+Fluffy.ResearchTree.CLClickMoveToFrontOfQueue</t>
@@ -155,6 +904,9 @@
     <t>Ctrl-Left-Click to move to front of queue</t>
   </si>
   <si>
+    <t>Ctrl-왼쪽 클릭으로 대기열의 맨 앞으로 보냅니다.</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.SLClickAddToQueue</t>
   </si>
   <si>
@@ -164,6 +916,9 @@
     <t>Shift-Left-Click to add to queue</t>
   </si>
   <si>
+    <t>Shift-왼쪽 클릭으로 대기열에 추가합니다</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.CLClickAddToFrontOfQueue</t>
   </si>
   <si>
@@ -173,6 +928,9 @@
     <t>Ctrl-Left-Click to add to front of queue</t>
   </si>
   <si>
+    <t>Ctrl-왼쪽 클릭으로 대기열의 맨 앞에 추가합니다.</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.SRClickShowInfo</t>
   </si>
   <si>
@@ -182,6 +940,9 @@
     <t>Right-Click to show info-window</t>
   </si>
   <si>
+    <t>오른쪽 클릭으로 정보창을 엽니다.</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.CannotMoveMore</t>
   </si>
   <si>
@@ -191,6 +952,9 @@
     <t>{0} cannot be moved more to the front of the queue than it already is</t>
   </si>
   <si>
+    <t>더 이상 {0}을/를 대기열 앞으로 옮길 수 없습니다</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.RClickInstaFinish</t>
   </si>
   <si>
@@ -200,6 +964,9 @@
     <t>(DEBUG) Right-Click to finish instantly</t>
   </si>
   <si>
+    <t>(DEBUG) 우클릭으로 즉시 연구 완료</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.RClickInstaFinishNew</t>
   </si>
   <si>
@@ -209,6 +976,9 @@
     <t>(DEBUG) Shift-Rightclick to finish instantly</t>
   </si>
   <si>
+    <t>(DEBUG) Shift-우클릭으로 즉시 연구 완료</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.Requires</t>
   </si>
   <si>
@@ -218,6 +988,9 @@
     <t>Requires</t>
   </si>
   <si>
+    <t>MainButtonDef+FluffyResearchTree.description</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.NotStarted</t>
   </si>
   <si>
@@ -227,6 +1000,9 @@
     <t>Not started, costs {0}</t>
   </si>
   <si>
+    <t>시작되지 않음: {0} 필요</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.InProgress</t>
   </si>
   <si>
@@ -236,6 +1012,9 @@
     <t>In progress, {0} of {1} done</t>
   </si>
   <si>
+    <t>진행 중: {0}/{1} 완료</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.LeadsTo</t>
   </si>
   <si>
@@ -245,6 +1024,9 @@
     <t>Leads to</t>
   </si>
   <si>
+    <t>FluffyResearchTree.label</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.StorytellerDoesNotAllow</t>
   </si>
   <si>
@@ -254,6 +1036,9 @@
     <t>Storyteller does not allow this tech</t>
   </si>
   <si>
+    <t>이야기꾼으로 인해 제한된 기술입니다.</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.RimedievalDoesNotAllow</t>
   </si>
   <si>
@@ -263,6 +1048,9 @@
     <t>Rimedieval settings does not allow this tech</t>
   </si>
   <si>
+    <t>Rimedieval으로 인해 제한된 기술입니다.</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.None</t>
   </si>
   <si>
@@ -272,6 +1060,9 @@
     <t>none</t>
   </si>
   <si>
+    <t>없음</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.ShowCompletion</t>
   </si>
   <si>
@@ -281,6 +1072,9 @@
     <t>Show completion message for finished research</t>
   </si>
   <si>
+    <t>연구가 완료되면 완료 메시지를 보냅니다</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.StillLoading</t>
   </si>
   <si>
@@ -290,6 +1084,9 @@
     <t>Tree is loading for the first time, this can take a while</t>
   </si>
   <si>
+    <t>연구 목록을 처음 로드하는 중입니다. 시간이 걸릴 수 있습니다.</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.CurrentModVersion</t>
   </si>
   <si>
@@ -299,6 +1096,9 @@
     <t>Installed mod-version: {0}</t>
   </si>
   <si>
+    <t>현재 모드 버전: {0}</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.PauseOnOpen</t>
   </si>
   <si>
@@ -308,6 +1108,9 @@
     <t>Pause game on opening research-tree</t>
   </si>
   <si>
+    <t>표시 중 일시정지</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.VanillaGraphics</t>
   </si>
   <si>
@@ -320,12 +1123,18 @@
     <t>Keyed+Fluffy.ResearchTree.LoadType</t>
   </si>
   <si>
+    <t>Shift-Click to remove from queue</t>
+  </si>
+  <si>
     <t>Fluffy.ResearchTree.LoadType</t>
   </si>
   <si>
     <t>When should the research-tree get generated?</t>
   </si>
   <si>
+    <t>연구 트리가 생성되는 시간 선택</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.LoadTypeOne</t>
   </si>
   <si>
@@ -335,6 +1144,9 @@
     <t>During game load</t>
   </si>
   <si>
+    <t>게임 로딩 동안</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.LoadTypeTwo</t>
   </si>
   <si>
@@ -344,6 +1156,9 @@
     <t>After game load in background</t>
   </si>
   <si>
+    <t>게임 로딩 이후 백그라운드에서</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.LoadTypeThree</t>
   </si>
   <si>
@@ -353,6 +1168,9 @@
     <t>First time opening research-tree</t>
   </si>
   <si>
+    <t>연구창에 처음 들어갈 때</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.QueuedNode</t>
   </si>
   <si>
@@ -362,6 +1180,9 @@
     <t>Already queued node</t>
   </si>
   <si>
+    <t>해당 연구가 이미 대기열에 존재합니다.</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.MissingFacilities</t>
   </si>
   <si>
@@ -371,6 +1192,9 @@
     <t>Missing {0}</t>
   </si>
   <si>
+    <t>{0} 필요</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.MissingTechprints</t>
   </si>
   <si>
@@ -380,6 +1204,9 @@
     <t>Insufficient techprints {0}/{1}</t>
   </si>
   <si>
+    <t>기술 청사진 필요: {0}/{1}</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.MissingStudiedThings</t>
   </si>
   <si>
@@ -389,6 +1216,9 @@
     <t>Missing item-studies: {0}</t>
   </si>
   <si>
+    <t>대상 연구 필요: {0}</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.MissingMechanitorRequirement</t>
   </si>
   <si>
@@ -398,6 +1228,9 @@
     <t>Missing mechanitor</t>
   </si>
   <si>
+    <t>메카나이터 필요</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.NoResearchFound</t>
   </si>
   <si>
@@ -407,6 +1240,9 @@
     <t>no research found</t>
   </si>
   <si>
+    <t>검색 결과 없음</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.NothingQueued</t>
   </si>
   <si>
@@ -416,6 +1252,9 @@
     <t>no research queued</t>
   </si>
   <si>
+    <t>대기열에 연구 없음</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.NextInQueue</t>
   </si>
   <si>
@@ -425,6 +1264,9 @@
     <t>Next in queue: {0}</t>
   </si>
   <si>
+    <t>대기열에 있는 다음 연구: {0}</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.PreparingTree.Setup</t>
   </si>
   <si>
@@ -434,6 +1276,9 @@
     <t>Preparing research nodes</t>
   </si>
   <si>
+    <t>연구 노드 준비 중</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.PreparingTree.CrossingReduction</t>
   </si>
   <si>
@@ -443,6 +1288,9 @@
     <t>Reducing crossings</t>
   </si>
   <si>
+    <t>교차 노드 정렬하는 중</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.PreparingTree.Layout</t>
   </si>
   <si>
@@ -452,6 +1300,9 @@
     <t>Finalizing layout</t>
   </si>
   <si>
+    <t>레이아웃 마무리 중</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.PreparingTree.LayoutNew</t>
   </si>
   <si>
@@ -461,6 +1312,9 @@
     <t>Finalizing research tree layout</t>
   </si>
   <si>
+    <t>연구 트리 레이아웃 마무리 중</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.RestoreQueue</t>
   </si>
   <si>
@@ -470,6 +1324,9 @@
     <t>Restoring queue</t>
   </si>
   <si>
+    <t>대기열 복원</t>
+  </si>
+  <si>
     <t>Keyed+ResearchPal.BuildingResearchTreeAsync</t>
   </si>
   <si>
@@ -488,6 +1345,9 @@
     <t>Use Ctrl to vertically scroll the research-tree</t>
   </si>
   <si>
+    <t>Ctrl 키를 세로 스크롤에 사용</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.CtrlFunctionZoom</t>
   </si>
   <si>
@@ -497,6 +1357,9 @@
     <t>Use Ctrl to zoom the research-tree</t>
   </si>
   <si>
+    <t>Ctrl 키를 연구창 확대/축소에 사용</t>
+  </si>
+  <si>
     <t>Keyed+Fluffy.ResearchTree.ResolutionChange</t>
   </si>
   <si>
@@ -504,6 +1367,9 @@
   </si>
   <si>
     <t>ResearchTree: Graphic-change detected, research tree will be regenerated</t>
+  </si>
+  <si>
+    <t>ResearchTree: 그래픽 변경이 감지되면 연구 트리가 다시 생성됩니다.</t>
   </si>
   <si>
     <t>Keyed+Fluffy.ResearchTree.UIScaleWarning</t>
@@ -520,152 +1386,204 @@
 이 문제가 발생하면 '연구창에 처음 들어갈 때' 옵션을 사용하세요.</t>
   </si>
   <si>
-    <t>ResearchTree: 그래픽 변경이 감지되면 연구 트리가 다시 생성됩니다.</t>
-  </si>
-  <si>
-    <t>Ctrl 키를 연구창 확대/축소에 사용</t>
-  </si>
-  <si>
-    <t>Ctrl 키를 세로 스크롤에 사용</t>
-  </si>
-  <si>
-    <t>대기열 복원</t>
-  </si>
-  <si>
-    <t>연구 트리 레이아웃 마무리 중</t>
-  </si>
-  <si>
-    <t>레이아웃 마무리 중</t>
-  </si>
-  <si>
-    <t>교차 노드 정렬하는 중</t>
-  </si>
-  <si>
-    <t>연구 노드 준비 중</t>
-  </si>
-  <si>
-    <t>대기열에 있는 다음 연구: {0}</t>
-  </si>
-  <si>
-    <t>대기열에 연구 없음</t>
-  </si>
-  <si>
-    <t>검색 결과 없음</t>
-  </si>
-  <si>
-    <t>메카나이터 필요</t>
-  </si>
-  <si>
-    <t>대상 연구 필요: {0}</t>
-  </si>
-  <si>
-    <t>기술 청사진 필요: {0}/{1}</t>
-  </si>
-  <si>
-    <t>{0} 필요</t>
-  </si>
-  <si>
-    <t>해당 연구가 이미 대기열에 존재합니다.</t>
-  </si>
-  <si>
-    <t>연구창에 처음 들어갈 때</t>
-  </si>
-  <si>
-    <t>게임 로딩 이후 백그라운드에서</t>
-  </si>
-  <si>
-    <t>게임 로딩 동안</t>
-  </si>
-  <si>
-    <t>연구 트리가 생성되는 시간 선택</t>
-  </si>
-  <si>
-    <t>표시 중 일시정지</t>
-  </si>
-  <si>
-    <t>현재 모드 버전: {0}</t>
-  </si>
-  <si>
-    <t>연구 목록을 처음 로드하는 중입니다. 시간이 걸릴 수 있습니다.</t>
-  </si>
-  <si>
-    <t>연구가 완료되면 완료 메시지를 보냅니다</t>
-  </si>
-  <si>
-    <t>없음</t>
-  </si>
-  <si>
-    <t>Rimedieval으로 인해 제한된 기술입니다.</t>
-  </si>
-  <si>
-    <t>이야기꾼으로 인해 제한된 기술입니다.</t>
-  </si>
-  <si>
-    <t>선행 기술</t>
-  </si>
-  <si>
-    <t>진행 중: {0}/{1} 완료</t>
-  </si>
-  <si>
-    <t>시작되지 않음: {0} 필요</t>
-  </si>
-  <si>
-    <t>요구 사항</t>
-  </si>
-  <si>
-    <t>(DEBUG) Shift-우클릭으로 즉시 연구 완료</t>
-  </si>
-  <si>
-    <t>(DEBUG) 우클릭으로 즉시 연구 완료</t>
-  </si>
-  <si>
-    <t>더 이상 {0}을/를 대기열 앞으로 옮길 수 없습니다</t>
-  </si>
-  <si>
-    <t>오른쪽 클릭으로 정보창을 엽니다.</t>
-  </si>
-  <si>
-    <t>Ctrl-왼쪽 클릭으로 대기열의 맨 앞에 추가합니다.</t>
-  </si>
-  <si>
-    <t>Shift-왼쪽 클릭으로 대기열에 추가합니다</t>
-  </si>
-  <si>
-    <t>Ctrl-왼쪽 클릭으로 대기열의 맨 앞으로 보냅니다.</t>
-  </si>
-  <si>
-    <t>왼쪽 클릭으로 대기열에서 제거합니다.</t>
-  </si>
-  <si>
-    <t>왼쪽 클릭으로 대기열을 변경합니다.</t>
-  </si>
-  <si>
-    <t>{0} 재배 가능</t>
-  </si>
-  <si>
-    <t>{0} 레시피 사용 가능</t>
-  </si>
-  <si>
-    <t>{0} 건설 사용 가능</t>
+    <t>Hold SHIFT to open the vanilla research window</t>
+  </si>
+  <si>
+    <t>Keyed+Fluffy.ResearchTree.HoldForNew</t>
+  </si>
+  <si>
+    <t>Fluffy.ResearchTree.HoldForNew</t>
+  </si>
+  <si>
+    <t>Hold SHIFT to open the new research window</t>
+  </si>
+  <si>
+    <t>Keyed+Fluffy.ResearchTree.VerboseLogging</t>
+  </si>
+  <si>
+    <t>Fluffy.ResearchTree.VerboseLogging</t>
+  </si>
+  <si>
+    <t>Verbose logging</t>
+  </si>
+  <si>
+    <t>Keyed+Fluffy.ResearchTree.NoIdeologyPopup</t>
+  </si>
+  <si>
+    <t>Fluffy.ResearchTree.NoIdeologyPopup</t>
+  </si>
+  <si>
+    <t>Do not show missing meme-warning</t>
+  </si>
+  <si>
+    <t>Keyed+Fluffy.ResearchTree.NoIdeologyPopupTT</t>
+  </si>
+  <si>
+    <t>Fluffy.ResearchTree.NoIdeologyPopupTT</t>
+  </si>
+  <si>
+    <t>When selecting a research, the popup warning that it will unlock items that your current Ideology does not allow will not be shown</t>
+  </si>
+  <si>
+    <t>Keyed+Fluffy.ResearchTree.GrimworldDoesNotAllow</t>
+  </si>
+  <si>
+    <t>Fluffy.ResearchTree.GrimworldDoesNotAllow</t>
+  </si>
+  <si>
+    <t>Grimworld study requirement not fulfilled, right click to show detailed info</t>
+  </si>
+  <si>
+    <t>Keyed+Fluffy.ResearchTree.SemiRandomResearchLoaded</t>
+  </si>
+  <si>
+    <t>Fluffy.ResearchTree.SemiRandomResearchLoaded</t>
+  </si>
+  <si>
+    <t>Semi Random Research does not allow choosing research freely</t>
+  </si>
+  <si>
+    <t>Keyed+Fluffy.ResearchTree.Reset</t>
+  </si>
+  <si>
+    <t>Fluffy.ResearchTree.Reset</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>Keyed+Fluffy.ResearchTree.ResetLabel</t>
+  </si>
+  <si>
+    <t>Fluffy.ResearchTree.ResetLabel</t>
+  </si>
+  <si>
+    <t>Reset all settings</t>
+  </si>
+  <si>
+    <t>Keyed+Fluffy.ResearchTree.LoadingWait</t>
+  </si>
+  <si>
+    <t>Fluffy.ResearchTree.LoadingWait</t>
+  </si>
+  <si>
+    <t>Tree not finished generating, click to open vanilla tree</t>
+  </si>
+  <si>
+    <t>Keyed+Fluffy.ResearchTree.LoadTypeFour</t>
+  </si>
+  <si>
+    <t>Fluffy.ResearchTree.LoadTypeFour</t>
+  </si>
+  <si>
+    <t>Do not generate research tree, but keep research queue</t>
+  </si>
+  <si>
+    <t>Keyed+Fluffy.ResearchTree.OverrideResearch</t>
+  </si>
+  <si>
+    <t>Fluffy.ResearchTree.OverrideResearch</t>
+  </si>
+  <si>
+    <t>Make the research tree as default research tab \n(hold shift for open vanilla)</t>
+  </si>
+  <si>
+    <t>Patches.MainButtonDef+BetterResearchTab.label</t>
+  </si>
+  <si>
+    <t>Patches.MainButtonDef</t>
+  </si>
+  <si>
+    <t>BetterResearchTab.label</t>
+  </si>
+  <si>
+    <t>##packageId##andery233xj.mod.BetterResearchTabs</t>
+  </si>
+  <si>
+    <t>Patches.MainButtonDef+BetterResearchTab.description</t>
+  </si>
+  <si>
+    <t>BetterResearchTab.description</t>
+  </si>
+  <si>
+    <t>Patches.MainButtonDef+OrganizedResearchTab.label</t>
+  </si>
+  <si>
+    <t>OrganizedResearchTab.label</t>
+  </si>
+  <si>
+    <t>##packageId##Mlie.OrganizedResearchTab</t>
+  </si>
+  <si>
+    <t>Patches.MainButtonDef+OrganizedResearchTab.description</t>
+  </si>
+  <si>
+    <t>OrganizedResearchTab.description</t>
+  </si>
+  <si>
+    <t>연구</t>
+  </si>
+  <si>
+    <t>가능한 연구 목록을 확인하고 연구과제를 정합니다.\n\nShift+클릭으로 기본 연구 UI를 열 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>가능한 연구 목록을 확인하고 연구과제를 정합니다.</t>
   </si>
   <si>
-    <t>연구</t>
-  </si>
-  <si>
-    <t>가능한 연구 목록을 확인하고 연구과제를 정합니다.\n\nShift+클릭으로 기본 연구 UI를 열 수 있습니다.</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>{0}(을)를 {1}에 심기 가능</t>
+    <t>연구 트리 생성 중</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>이전 그래픽 방식 사용 (깜박이는 경우)</t>
+    <t>SHIFT 키로 기본 연구 화면을 엽니다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SHIFT 키로 신규 연구 화면을 엽니다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>세부 기록</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>연구를 선택할 때 현재 사상에서 허용하지 않는 아이템이 잠금 해제된다는 팝업 경고가 표시되지 않습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사상 경고 표시 안함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Grimworld 연구 요구 사항이 충족되지 않았습니다. 자세한 정보를 보려면 마우스 오른쪽 버튼을 클릭하십시오.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Semi Random Research는 연구를 자유롭게 선택할 수 없습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>초기화</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 설정 초기화</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>연구 트리를 생성하지 않고 연구 대기열만 사용합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>연구 트리를 기본 연구 탭으로 사용\n(Shift+클릭으로 기본 연구 화면 사용 가능)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>연구 트리 생성이 완료되지 않았습니다. 기본 연구 화면을 열려면 클릭하세요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shift+클릭으로 대기열에서 제거합니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -673,7 +1591,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -692,13 +1610,41 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -713,9 +1659,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1017,11 +1966,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1032,7 +1981,8 @@
     <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.6328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="36.7265625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -1065,865 +2015,1163 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>206</v>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>204</v>
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>203</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>202</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>208</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>201</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>200</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>199</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>198</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>197</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>196</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>195</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>194</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>193</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>192</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>191</v>
+        <v>74</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>190</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>189</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>188</v>
+        <v>86</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>187</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>186</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>185</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>184</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>183</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>182</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>181</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>209</v>
+        <v>118</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>180</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>178</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>176</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>114</v>
+        <v>147</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>174</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>119</v>
+        <v>154</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>121</v>
+        <v>157</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>123</v>
+        <v>159</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>131</v>
+        <v>170</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>133</v>
+        <v>173</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>134</v>
+        <v>174</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>135</v>
+        <v>175</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>136</v>
+        <v>177</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>139</v>
+        <v>181</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>141</v>
+        <v>183</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>142</v>
+        <v>185</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>143</v>
+        <v>186</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>144</v>
+        <v>187</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>145</v>
+        <v>189</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>146</v>
+        <v>190</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>147</v>
+        <v>191</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>207</v>
+        <v>256</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>148</v>
+        <v>192</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>149</v>
+        <v>193</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>150</v>
+        <v>194</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>163</v>
+        <v>195</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>151</v>
+        <v>196</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>152</v>
+        <v>197</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>153</v>
+        <v>198</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>162</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>154</v>
+        <v>200</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>155</v>
+        <v>201</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>156</v>
+        <v>202</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>161</v>
+        <v>203</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>157</v>
+        <v>204</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A54" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>160</v>
+      <c r="F69" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>